<commit_message>
nuevo equipo de trabajo
</commit_message>
<xml_diff>
--- a/Articulos/Apertura2012-Apertura2021_LigaMX_30-11-2021.xlsx
+++ b/Articulos/Apertura2012-Apertura2021_LigaMX_30-11-2021.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\La Cima del Éxito\Futbol\articulos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\La Cima del Éxito\Futbol\Articulos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{32182446-CB1B-464D-8E64-7977530C5AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27214E27-9D96-4B50-BA06-45F4B68A269B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Apertura2012-Apertura2021_LigaM" sheetId="1" r:id="rId1"/>
     <sheet name="Goals%" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="100">
   <si>
     <t>team</t>
   </si>
@@ -300,6 +299,39 @@
   </si>
   <si>
     <t>PP100m</t>
+  </si>
+  <si>
+    <t>Pumas</t>
+  </si>
+  <si>
+    <t>América</t>
+  </si>
+  <si>
+    <t>Mazatlán</t>
+  </si>
+  <si>
+    <t>Santos</t>
+  </si>
+  <si>
+    <t>León</t>
+  </si>
+  <si>
+    <t>Juárez</t>
+  </si>
+  <si>
+    <t>Tigres</t>
+  </si>
+  <si>
+    <t>Querétaro</t>
+  </si>
+  <si>
+    <t>Tijuana</t>
+  </si>
+  <si>
+    <t>Chivas</t>
+  </si>
+  <si>
+    <t>Dorados</t>
   </si>
 </sst>
 </file>
@@ -811,14 +843,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -871,13 +902,22 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -934,25 +974,16 @@
       </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -2458,13 +2489,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:BK27" totalsRowCount="1">
-  <autoFilter ref="A1:BK26" xr:uid="{00000000-0009-0000-0100-000001000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Guadalajara Chivas"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:BK26" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:BK26">
     <sortCondition descending="1" ref="C1:C26"/>
   </sortState>
@@ -2474,42 +2499,42 @@
     <tableColumn id="64" xr3:uid="{47306BBB-92C6-40E0-B742-1A09942C7F87}" name="PP100m" dataDxfId="8">
       <calculatedColumnFormula>(Table1[[#This Row],[rWins]]*3+Table1[[#This Row],[rDraws]])*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="rPoints" totalsRowDxfId="7" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="rPoints" totalsRowDxfId="3" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>Table1[[#This Row],[Points]]/Table1[[#This Row],[xPoints]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Points" totalsRowFunction="custom">
       <totalsRowFormula>SUM(Table1[Points])</totalsRowFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="xPoints" totalsRowFunction="sum"/>
-    <tableColumn id="61" xr3:uid="{E4842FD8-02B0-423B-8143-EFCC3761281A}" name="Matches" totalsRowFunction="sum" dataDxfId="6">
+    <tableColumn id="61" xr3:uid="{E4842FD8-02B0-423B-8143-EFCC3761281A}" name="Matches" totalsRowFunction="sum" dataDxfId="7">
       <calculatedColumnFormula>Table1[[#This Row],[Wins]]+Table1[[#This Row],[Draws]]+Table1[[#This Row],[Losses]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="rWins" totalsRowDxfId="5" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="rWins" totalsRowDxfId="2" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>Table1[[#This Row],[Wins]]/Table1[[#This Row],[xWins]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Wins" totalsRowFunction="sum"/>
-    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0000-000037000000}" name="rDraws" totalsRowDxfId="4" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0000-000037000000}" name="rDraws" totalsRowDxfId="1" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>Table1[[#This Row],[Draws]]/Table1[[#This Row],[xDraws]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Draws" totalsRowFunction="sum"/>
-    <tableColumn id="56" xr3:uid="{00000000-0010-0000-0000-000038000000}" name="rLosses" totalsRowDxfId="3" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="56" xr3:uid="{00000000-0010-0000-0000-000038000000}" name="rLosses" totalsRowDxfId="0" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>Table1[[#This Row],[Losses]]/Table1[[#This Row],[xLosses]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Losses" totalsRowFunction="sum"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="xWins" totalsRowFunction="sum"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="xDraws" totalsRowFunction="sum"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="xLosses" totalsRowFunction="sum"/>
-    <tableColumn id="60" xr3:uid="{00000000-0010-0000-0000-00003C000000}" name="GD_Diff" dataDxfId="2">
+    <tableColumn id="60" xr3:uid="{00000000-0010-0000-0000-00003C000000}" name="GD_Diff" dataDxfId="6">
       <calculatedColumnFormula>Table1[[#This Row],[GoalsF_Diff]]+Table1[[#This Row],[GoalsA_Diff]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="GD"/>
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="xGoalDiff"/>
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="GoalsF_Diff"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="GoalsA_Diff"/>
-    <tableColumn id="63" xr3:uid="{0777CA56-3747-45B3-9510-EA6AB350BBD4}" name="GPT" dataDxfId="1">
+    <tableColumn id="63" xr3:uid="{0777CA56-3747-45B3-9510-EA6AB350BBD4}" name="GPT" dataDxfId="5">
       <calculatedColumnFormula>Table1[[#This Row],[GPM]]*17</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="62" xr3:uid="{2B29B01E-DE7E-471B-987C-399AA1026D30}" name="GPM" dataDxfId="0">
+    <tableColumn id="62" xr3:uid="{2B29B01E-DE7E-471B-987C-399AA1026D30}" name="GPM" dataDxfId="4">
       <calculatedColumnFormula>Table1[[#This Row],[GoalsF]]/Table1[[#This Row],[Matches]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="58" xr3:uid="{00000000-0010-0000-0000-00003A000000}" name="rGoalsF" dataCellStyle="Percent">
@@ -2860,9 +2885,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BK34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O28" sqref="O28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2965,10 +2990,10 @@
       <c r="U1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="V1" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="W1" s="6" t="s">
         <v>86</v>
       </c>
       <c r="X1" s="2" t="s">
@@ -3092,14 +3117,14 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:63" hidden="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:63" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C2" s="9">
+        <v>90</v>
+      </c>
+      <c r="C2" s="8">
         <f>(Table1[[#This Row],[rWins]]*3+Table1[[#This Row],[rDraws]])*100</f>
         <v>430.67187052224705</v>
       </c>
@@ -3167,7 +3192,7 @@
         <f>Table1[[#This Row],[GPM]]*17</f>
         <v>26.921135646687695</v>
       </c>
-      <c r="W2" s="8">
+      <c r="W2" s="7">
         <f>Table1[[#This Row],[GoalsF]]/Table1[[#This Row],[Matches]]</f>
         <v>1.5835962145110409</v>
       </c>
@@ -3294,14 +3319,14 @@
         <v>36.033292417389603</v>
       </c>
     </row>
-    <row r="3" spans="1:63" hidden="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>15</v>
       </c>
       <c r="B3" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <f>(Table1[[#This Row],[rWins]]*3+Table1[[#This Row],[rDraws]])*100</f>
         <v>427.93412683553396</v>
       </c>
@@ -3369,7 +3394,7 @@
         <f>Table1[[#This Row],[GPM]]*17</f>
         <v>23.917981072555204</v>
       </c>
-      <c r="W3" s="8">
+      <c r="W3" s="7">
         <f>Table1[[#This Row],[GoalsF]]/Table1[[#This Row],[Matches]]</f>
         <v>1.4069400630914826</v>
       </c>
@@ -3496,14 +3521,14 @@
         <v>33.633085032618403</v>
       </c>
     </row>
-    <row r="4" spans="1:63" hidden="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="9">
+        <v>89</v>
+      </c>
+      <c r="C4" s="8">
         <f>(Table1[[#This Row],[rWins]]*3+Table1[[#This Row],[rDraws]])*100</f>
         <v>422.40453755761666</v>
       </c>
@@ -3571,7 +3596,7 @@
         <f>Table1[[#This Row],[GPM]]*17</f>
         <v>21.933753943217667</v>
       </c>
-      <c r="W4" s="8">
+      <c r="W4" s="7">
         <f>Table1[[#This Row],[GoalsF]]/Table1[[#This Row],[Matches]]</f>
         <v>1.2902208201892744</v>
       </c>
@@ -3698,14 +3723,14 @@
         <v>32.640514176275602</v>
       </c>
     </row>
-    <row r="5" spans="1:63" hidden="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <f>(Table1[[#This Row],[rWins]]*3+Table1[[#This Row],[rDraws]])*100</f>
         <v>418.1793700968197</v>
       </c>
@@ -3773,7 +3798,7 @@
         <f>Table1[[#This Row],[GPM]]*17</f>
         <v>19.252365930599371</v>
       </c>
-      <c r="W5" s="8">
+      <c r="W5" s="7">
         <f>Table1[[#This Row],[GoalsF]]/Table1[[#This Row],[Matches]]</f>
         <v>1.1324921135646688</v>
       </c>
@@ -3900,14 +3925,14 @@
         <v>30.7861353046499</v>
       </c>
     </row>
-    <row r="6" spans="1:63" hidden="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:63" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>22</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <f>(Table1[[#This Row],[rWins]]*3+Table1[[#This Row],[rDraws]])*100</f>
         <v>415.99351337183953</v>
       </c>
@@ -3975,7 +4000,7 @@
         <f>Table1[[#This Row],[GPM]]*17</f>
         <v>23.390977443609025</v>
       </c>
-      <c r="W6" s="8">
+      <c r="W6" s="7">
         <f>Table1[[#This Row],[GoalsF]]/Table1[[#This Row],[Matches]]</f>
         <v>1.3759398496240602</v>
       </c>
@@ -4102,14 +4127,14 @@
         <v>27.4210357098471</v>
       </c>
     </row>
-    <row r="7" spans="1:63" hidden="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:63" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="9">
+        <v>91</v>
+      </c>
+      <c r="C7" s="8">
         <f>(Table1[[#This Row],[rWins]]*3+Table1[[#This Row],[rDraws]])*100</f>
         <v>415.17910679170899</v>
       </c>
@@ -4177,7 +4202,7 @@
         <f>Table1[[#This Row],[GPM]]*17</f>
         <v>20.333333333333332</v>
       </c>
-      <c r="W7" s="8">
+      <c r="W7" s="7">
         <f>Table1[[#This Row],[GoalsF]]/Table1[[#This Row],[Matches]]</f>
         <v>1.196078431372549</v>
       </c>
@@ -4304,14 +4329,14 @@
         <v>4.8536312068882399</v>
       </c>
     </row>
-    <row r="8" spans="1:63" hidden="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:63" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>17</v>
       </c>
       <c r="B8" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="8">
         <f>(Table1[[#This Row],[rWins]]*3+Table1[[#This Row],[rDraws]])*100</f>
         <v>413.66801570608612</v>
       </c>
@@ -4379,7 +4404,7 @@
         <f>Table1[[#This Row],[GPM]]*17</f>
         <v>21.320441988950275</v>
       </c>
-      <c r="W8" s="8">
+      <c r="W8" s="7">
         <f>Table1[[#This Row],[GoalsF]]/Table1[[#This Row],[Matches]]</f>
         <v>1.2541436464088398</v>
       </c>
@@ -4506,14 +4531,14 @@
         <v>18.552106399119399</v>
       </c>
     </row>
-    <row r="9" spans="1:63" hidden="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:63" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="9">
+        <v>92</v>
+      </c>
+      <c r="C9" s="8">
         <f>(Table1[[#This Row],[rWins]]*3+Table1[[#This Row],[rDraws]])*100</f>
         <v>413.03381313580098</v>
       </c>
@@ -4581,7 +4606,7 @@
         <f>Table1[[#This Row],[GPM]]*17</f>
         <v>24.50788643533123</v>
       </c>
-      <c r="W9" s="8">
+      <c r="W9" s="7">
         <f>Table1[[#This Row],[GoalsF]]/Table1[[#This Row],[Matches]]</f>
         <v>1.4416403785488958</v>
       </c>
@@ -4708,14 +4733,14 @@
         <v>34.283464191267797</v>
       </c>
     </row>
-    <row r="10" spans="1:63" hidden="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:63" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="9">
         <f>(Table1[[#This Row],[rWins]]*3+Table1[[#This Row],[rDraws]])*100</f>
         <v>406.05583011938666</v>
       </c>
@@ -4783,7 +4808,7 @@
         <f>Table1[[#This Row],[GPM]]*17</f>
         <v>21.2</v>
       </c>
-      <c r="W10" s="8">
+      <c r="W10" s="7">
         <f>Table1[[#This Row],[GoalsF]]/Table1[[#This Row],[Matches]]</f>
         <v>1.2470588235294118</v>
       </c>
@@ -4910,14 +4935,14 @@
         <v>16.888895535430201</v>
       </c>
     </row>
-    <row r="11" spans="1:63" hidden="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:63" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C11" s="9">
+        <v>93</v>
+      </c>
+      <c r="C11" s="8">
         <f>(Table1[[#This Row],[rWins]]*3+Table1[[#This Row],[rDraws]])*100</f>
         <v>402.40770188654642</v>
       </c>
@@ -4985,7 +5010,7 @@
         <f>Table1[[#This Row],[GPM]]*17</f>
         <v>26.921135646687695</v>
       </c>
-      <c r="W11" s="8">
+      <c r="W11" s="7">
         <f>Table1[[#This Row],[GoalsF]]/Table1[[#This Row],[Matches]]</f>
         <v>1.5835962145110409</v>
       </c>
@@ -5112,14 +5137,14 @@
         <v>34.823760677035601</v>
       </c>
     </row>
-    <row r="12" spans="1:63" hidden="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:63" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>13</v>
       </c>
       <c r="B12" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="8">
         <f>(Table1[[#This Row],[rWins]]*3+Table1[[#This Row],[rDraws]])*100</f>
         <v>400.71535313336074</v>
       </c>
@@ -5187,7 +5212,7 @@
         <f>Table1[[#This Row],[GPM]]*17</f>
         <v>23.542586750788644</v>
       </c>
-      <c r="W12" s="8">
+      <c r="W12" s="7">
         <f>Table1[[#This Row],[GoalsF]]/Table1[[#This Row],[Matches]]</f>
         <v>1.3848580441640379</v>
       </c>
@@ -5314,14 +5339,14 @@
         <v>35.585194916308303</v>
       </c>
     </row>
-    <row r="13" spans="1:63" hidden="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:63" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="9">
+        <v>94</v>
+      </c>
+      <c r="C13" s="8">
         <f>(Table1[[#This Row],[rWins]]*3+Table1[[#This Row],[rDraws]])*100</f>
         <v>400.00280524519337</v>
       </c>
@@ -5389,7 +5414,7 @@
         <f>Table1[[#This Row],[GPM]]*17</f>
         <v>17.215189873417721</v>
       </c>
-      <c r="W13" s="8">
+      <c r="W13" s="7">
         <f>Table1[[#This Row],[GoalsF]]/Table1[[#This Row],[Matches]]</f>
         <v>1.0126582278481013</v>
       </c>
@@ -5516,14 +5541,14 @@
         <v>7.5205937071360101</v>
       </c>
     </row>
-    <row r="14" spans="1:63" hidden="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:63" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>69</v>
-      </c>
-      <c r="C14" s="9">
+        <v>95</v>
+      </c>
+      <c r="C14" s="8">
         <f>(Table1[[#This Row],[rWins]]*3+Table1[[#This Row],[rDraws]])*100</f>
         <v>398.19919077746044</v>
       </c>
@@ -5591,7 +5616,7 @@
         <f>Table1[[#This Row],[GPM]]*17</f>
         <v>25.044164037854888</v>
       </c>
-      <c r="W14" s="8">
+      <c r="W14" s="7">
         <f>Table1[[#This Row],[GoalsF]]/Table1[[#This Row],[Matches]]</f>
         <v>1.473186119873817</v>
       </c>
@@ -5718,14 +5743,14 @@
         <v>36.013992810418998</v>
       </c>
     </row>
-    <row r="15" spans="1:63" hidden="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:63" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>71</v>
-      </c>
-      <c r="C15" s="9">
+        <v>96</v>
+      </c>
+      <c r="C15" s="8">
         <f>(Table1[[#This Row],[rWins]]*3+Table1[[#This Row],[rDraws]])*100</f>
         <v>394.23904108293345</v>
       </c>
@@ -5793,7 +5818,7 @@
         <f>Table1[[#This Row],[GPM]]*17</f>
         <v>19.313291139240508</v>
       </c>
-      <c r="W15" s="8">
+      <c r="W15" s="7">
         <f>Table1[[#This Row],[GoalsF]]/Table1[[#This Row],[Matches]]</f>
         <v>1.1360759493670887</v>
       </c>
@@ -5920,14 +5945,14 @@
         <v>31.5024386148025</v>
       </c>
     </row>
-    <row r="16" spans="1:63" hidden="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:63" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>7</v>
       </c>
       <c r="B16" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="8">
         <f>(Table1[[#This Row],[rWins]]*3+Table1[[#This Row],[rDraws]])*100</f>
         <v>389.55136874284892</v>
       </c>
@@ -5995,7 +6020,7 @@
         <f>Table1[[#This Row],[GPM]]*17</f>
         <v>18.394321766561514</v>
       </c>
-      <c r="W16" s="8">
+      <c r="W16" s="7">
         <f>Table1[[#This Row],[GoalsF]]/Table1[[#This Row],[Matches]]</f>
         <v>1.0820189274447949</v>
       </c>
@@ -6122,14 +6147,14 @@
         <v>32.224152719653397</v>
       </c>
     </row>
-    <row r="17" spans="1:63" hidden="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:63" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="9">
+        <v>97</v>
+      </c>
+      <c r="C17" s="8">
         <f>(Table1[[#This Row],[rWins]]*3+Table1[[#This Row],[rDraws]])*100</f>
         <v>386.70839851656837</v>
       </c>
@@ -6197,7 +6222,7 @@
         <f>Table1[[#This Row],[GPM]]*17</f>
         <v>20.593059936908517</v>
       </c>
-      <c r="W17" s="8">
+      <c r="W17" s="7">
         <f>Table1[[#This Row],[GoalsF]]/Table1[[#This Row],[Matches]]</f>
         <v>1.2113564668769716</v>
       </c>
@@ -6324,14 +6349,14 @@
         <v>33.344443471061197</v>
       </c>
     </row>
-    <row r="18" spans="1:63" hidden="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:63" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>20</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="9">
         <f>(Table1[[#This Row],[rWins]]*3+Table1[[#This Row],[rDraws]])*100</f>
         <v>382.84029024819836</v>
       </c>
@@ -6399,7 +6424,7 @@
         <f>Table1[[#This Row],[GPM]]*17</f>
         <v>20.5</v>
       </c>
-      <c r="W18" s="8">
+      <c r="W18" s="7">
         <f>Table1[[#This Row],[GoalsF]]/Table1[[#This Row],[Matches]]</f>
         <v>1.2058823529411764</v>
       </c>
@@ -6526,14 +6551,14 @@
         <v>6.5244938787908797</v>
       </c>
     </row>
-    <row r="19" spans="1:63" hidden="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:63" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>9</v>
       </c>
       <c r="B19" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="8">
         <f>(Table1[[#This Row],[rWins]]*3+Table1[[#This Row],[rDraws]])*100</f>
         <v>381.65971263702556</v>
       </c>
@@ -6601,7 +6626,7 @@
         <f>Table1[[#This Row],[GPM]]*17</f>
         <v>25.794952681388011</v>
       </c>
-      <c r="W19" s="8">
+      <c r="W19" s="7">
         <f>Table1[[#This Row],[GoalsF]]/Table1[[#This Row],[Matches]]</f>
         <v>1.5173501577287065</v>
       </c>
@@ -6728,14 +6753,14 @@
         <v>35.310624487514502</v>
       </c>
     </row>
-    <row r="20" spans="1:63" hidden="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:63" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>3</v>
       </c>
       <c r="B20" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="8">
         <f>(Table1[[#This Row],[rWins]]*3+Table1[[#This Row],[rDraws]])*100</f>
         <v>380.74210863371627</v>
       </c>
@@ -6803,7 +6828,7 @@
         <f>Table1[[#This Row],[GPM]]*17</f>
         <v>23.381703470031546</v>
       </c>
-      <c r="W20" s="8">
+      <c r="W20" s="7">
         <f>Table1[[#This Row],[GoalsF]]/Table1[[#This Row],[Matches]]</f>
         <v>1.3753943217665616</v>
       </c>
@@ -6935,9 +6960,9 @@
         <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" s="9">
+        <v>98</v>
+      </c>
+      <c r="C21" s="8">
         <f>(Table1[[#This Row],[rWins]]*3+Table1[[#This Row],[rDraws]])*100</f>
         <v>380.72101120114547</v>
       </c>
@@ -7005,7 +7030,7 @@
         <f>Table1[[#This Row],[GPM]]*17</f>
         <v>18.876971608832807</v>
       </c>
-      <c r="W21" s="8">
+      <c r="W21" s="7">
         <f>Table1[[#This Row],[GoalsF]]/Table1[[#This Row],[Matches]]</f>
         <v>1.110410094637224</v>
       </c>
@@ -7132,14 +7157,14 @@
         <v>33.4117304416121</v>
       </c>
     </row>
-    <row r="22" spans="1:63" hidden="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:63" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>11</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="9">
         <f>(Table1[[#This Row],[rWins]]*3+Table1[[#This Row],[rDraws]])*100</f>
         <v>376.80148424974004</v>
       </c>
@@ -7207,7 +7232,7 @@
         <f>Table1[[#This Row],[GPM]]*17</f>
         <v>11.5</v>
       </c>
-      <c r="W22" s="8">
+      <c r="W22" s="7">
         <f>Table1[[#This Row],[GoalsF]]/Table1[[#This Row],[Matches]]</f>
         <v>0.67647058823529416</v>
       </c>
@@ -7334,14 +7359,14 @@
         <v>3.2649999486230801</v>
       </c>
     </row>
-    <row r="23" spans="1:63" hidden="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:63" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>18</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C23" s="10">
+      <c r="C23" s="9">
         <f>(Table1[[#This Row],[rWins]]*3+Table1[[#This Row],[rDraws]])*100</f>
         <v>371.13805966050063</v>
       </c>
@@ -7409,7 +7434,7 @@
         <f>Table1[[#This Row],[GPM]]*17</f>
         <v>15.927927927927927</v>
       </c>
-      <c r="W23" s="8">
+      <c r="W23" s="7">
         <f>Table1[[#This Row],[GoalsF]]/Table1[[#This Row],[Matches]]</f>
         <v>0.93693693693693691</v>
       </c>
@@ -7536,14 +7561,14 @@
         <v>20.524584494948801</v>
       </c>
     </row>
-    <row r="24" spans="1:63" hidden="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:63" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>16</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C24" s="10">
+        <v>99</v>
+      </c>
+      <c r="C24" s="9">
         <f>(Table1[[#This Row],[rWins]]*3+Table1[[#This Row],[rDraws]])*100</f>
         <v>344.04563667817894</v>
       </c>
@@ -7611,7 +7636,7 @@
         <f>Table1[[#This Row],[GPM]]*17</f>
         <v>15.5</v>
       </c>
-      <c r="W24" s="8">
+      <c r="W24" s="7">
         <f>Table1[[#This Row],[GoalsF]]/Table1[[#This Row],[Matches]]</f>
         <v>0.91176470588235292</v>
       </c>
@@ -7738,14 +7763,14 @@
         <v>3.08061424951639</v>
       </c>
     </row>
-    <row r="25" spans="1:63" hidden="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:63" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C25" s="8">
         <f>(Table1[[#This Row],[rWins]]*3+Table1[[#This Row],[rDraws]])*100</f>
         <v>340.22612200584905</v>
       </c>
@@ -7813,7 +7838,7 @@
         <f>Table1[[#This Row],[GPM]]*17</f>
         <v>18.366071428571427</v>
       </c>
-      <c r="W25" s="8">
+      <c r="W25" s="7">
         <f>Table1[[#This Row],[GoalsF]]/Table1[[#This Row],[Matches]]</f>
         <v>1.0803571428571428</v>
       </c>
@@ -7940,14 +7965,14 @@
         <v>10.8323557402882</v>
       </c>
     </row>
-    <row r="26" spans="1:63" hidden="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:63" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>4</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="10">
+      <c r="C26" s="9">
         <f>(Table1[[#This Row],[rWins]]*3+Table1[[#This Row],[rDraws]])*100</f>
         <v>331.85401605007058</v>
       </c>
@@ -8015,7 +8040,7 @@
         <f>Table1[[#This Row],[GPM]]*17</f>
         <v>19.5</v>
       </c>
-      <c r="W26" s="8">
+      <c r="W26" s="7">
         <f>Table1[[#This Row],[GoalsF]]/Table1[[#This Row],[Matches]]</f>
         <v>1.1470588235294117</v>
       </c>
@@ -8150,58 +8175,58 @@
       </c>
       <c r="F27">
         <f>SUBTOTAL(109,Table1[xPoints])</f>
-        <v>426.36669428563999</v>
+        <v>7810.7743785847169</v>
       </c>
       <c r="G27">
         <f>SUBTOTAL(109,Table1[Matches])</f>
-        <v>317</v>
+        <v>5722</v>
       </c>
       <c r="H27" s="1"/>
       <c r="I27">
         <f>SUBTOTAL(109,Table1[Wins])</f>
-        <v>99</v>
+        <v>2062</v>
       </c>
       <c r="J27" s="1"/>
       <c r="K27">
         <f>SUBTOTAL(109,Table1[Draws])</f>
-        <v>104</v>
+        <v>1598</v>
       </c>
       <c r="L27" s="1"/>
       <c r="M27">
         <f>SUBTOTAL(109,Table1[Losses])</f>
-        <v>114</v>
+        <v>2062</v>
       </c>
       <c r="N27">
         <f>SUBTOTAL(109,Table1[xWins])</f>
-        <v>112.30418951507301</v>
+        <v>2088.7743785847179</v>
       </c>
       <c r="O27">
         <f>SUBTOTAL(109,Table1[xDraws])</f>
-        <v>89.454125740420196</v>
+        <v>1544.4512428305497</v>
       </c>
       <c r="P27">
         <f>SUBTOTAL(109,Table1[xLosses])</f>
-        <v>115.241684744506</v>
+        <v>2088.7743785847197</v>
       </c>
       <c r="Y27">
         <f>SUBTOTAL(109,Table1[GoalsF])</f>
-        <v>352</v>
+        <v>7425</v>
       </c>
       <c r="Z27">
         <f>SUBTOTAL(109,Table1[xGoalsF])</f>
-        <v>401.79523544527802</v>
+        <v>7394.7242256684776</v>
       </c>
       <c r="AD27">
         <f>SUBTOTAL(109,Table1[HTGoalsF])</f>
-        <v>3</v>
+        <v>154</v>
       </c>
       <c r="AE27">
         <f>SUBTOTAL(109,Table1[xHTGoalsF])</f>
-        <v>176.05058489163801</v>
+        <v>3240.1340391149952</v>
       </c>
       <c r="BH27">
         <f>SUBTOTAL(109,Table1[xRCard])</f>
-        <v>33.641514865731502</v>
+        <v>600.01445613881663</v>
       </c>
     </row>
     <row r="29" spans="1:63" x14ac:dyDescent="0.45">
@@ -8249,9 +8274,9 @@
       </c>
       <c r="M31" s="1">
         <f>Table1[[#Totals],[Losses]]/Table1[[#Totals],[xLosses]]</f>
-        <v>0.98922538535202043</v>
-      </c>
-      <c r="Y31" s="6">
+        <v>0.98718177565790466</v>
+      </c>
+      <c r="Y31" s="1">
         <f>Y29/Z29</f>
         <v>1.0040942398130859</v>
       </c>
@@ -8273,7 +8298,7 @@
     <row r="34" spans="7:26" x14ac:dyDescent="0.45">
       <c r="G34">
         <f>Table1[[#Totals],[Matches]]/2</f>
-        <v>158.5</v>
+        <v>2861</v>
       </c>
       <c r="M34">
         <f>M33/19</f>
@@ -8352,8 +8377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>